<commit_message>
Replaced spring-boot-admin dependencies and fix report templates
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/evaluation-logs-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/evaluation-logs-report-template.xlsx
@@ -387,6 +387,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -395,9 +398,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -716,16 +716,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -751,15 +751,15 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -767,18 +767,18 @@
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -863,16 +863,16 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>

</xml_diff>

<commit_message>
Set sheet title in xls report templates
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/evaluation-logs-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/evaluation-logs-report-template.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="48" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Отчет по классификаторам" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Renamed requestStatus in xls reports
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/evaluation-logs-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/evaluation-logs-report-template.xlsx
@@ -166,9 +166,6 @@
     <t>${evaluationLog.requestId}</t>
   </si>
   <si>
-    <t>${evaluationLog.evaluationStatus}</t>
-  </si>
-  <si>
     <t>Классификатор</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
   </si>
   <si>
     <t>${evaluationLog.endDate}</t>
+  </si>
+  <si>
+    <t>${evaluationLog.requestStatus}</t>
   </si>
 </sst>
 </file>
@@ -805,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -820,10 +820,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -836,25 +836,25 @@
         <v>11</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="G7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>

</xml_diff>